<commit_message>
ajout de toutes les tables de la base de données sans relation
</commit_message>
<xml_diff>
--- a/DOCS/MERISE/Dictionnaire de données.xlsx
+++ b/DOCS/MERISE/Dictionnaire de données.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\80010-84-02\Desktop\CDA_20046-1\DOCS\MERISE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nastia/localhosts/fil-rouge/CDA_20046-1/DOCS/MERISE/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB1AB8B-2587-1D4A-BA05-EFEBA9125A2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="174">
   <si>
     <t>CODE</t>
   </si>
@@ -250,12 +251,6 @@
   </si>
   <si>
     <t>date de réception</t>
-  </si>
-  <si>
-    <t>quantity_delivered</t>
-  </si>
-  <si>
-    <t>quantité livrée</t>
   </si>
   <si>
     <t>payment_id</t>
@@ -552,8 +547,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -855,56 +850,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -915,6 +860,56 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1131,26 +1126,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.1640625" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1164,7 +1159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1174,11 +1169,11 @@
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1188,9 +1183,9 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:4" ht="15">
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1200,9 +1195,9 @@
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="1:4" ht="15">
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1212,11 +1207,11 @@
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -1226,9 +1221,9 @@
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" ht="15">
+      <c r="D6" s="29"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -1238,9 +1233,9 @@
       <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" ht="15">
+      <c r="D7" s="29"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
@@ -1250,9 +1245,9 @@
       <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" ht="15">
+      <c r="D8" s="29"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
@@ -1262,9 +1257,9 @@
       <c r="C9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" ht="15">
+      <c r="D9" s="29"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
@@ -1274,9 +1269,9 @@
       <c r="C10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="21"/>
-    </row>
-    <row r="11" spans="1:4" ht="15">
+      <c r="D10" s="29"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -1286,9 +1281,9 @@
       <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" ht="15">
+      <c r="D11" s="29"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
@@ -1298,9 +1293,9 @@
       <c r="C12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="1:4" ht="15">
+      <c r="D12" s="29"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>35</v>
       </c>
@@ -1310,9 +1305,9 @@
       <c r="C13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="22"/>
-    </row>
-    <row r="14" spans="1:4" ht="15">
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
@@ -1322,11 +1317,11 @@
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
@@ -1336,9 +1331,9 @@
       <c r="C15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:4" ht="15">
+      <c r="D15" s="29"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
@@ -1348,9 +1343,9 @@
       <c r="C16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1">
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -1360,9 +1355,9 @@
       <c r="C17" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" ht="15">
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -1372,9 +1367,9 @@
       <c r="C18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="22"/>
-    </row>
-    <row r="19" spans="1:4" ht="15">
+      <c r="D18" s="30"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
@@ -1388,7 +1383,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>55</v>
       </c>
@@ -1398,9 +1393,9 @@
       <c r="C20" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="21"/>
-    </row>
-    <row r="21" spans="1:4" ht="15">
+      <c r="D20" s="29"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>58</v>
       </c>
@@ -1410,9 +1405,9 @@
       <c r="C21" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="22"/>
-    </row>
-    <row r="22" spans="1:4" ht="15">
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>60</v>
       </c>
@@ -1422,11 +1417,11 @@
       <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>63</v>
       </c>
@@ -1436,9 +1431,9 @@
       <c r="C23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="36"/>
-    </row>
-    <row r="24" spans="1:4" ht="15">
+      <c r="D23" s="37"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>65</v>
       </c>
@@ -1448,9 +1443,9 @@
       <c r="C24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="36"/>
-    </row>
-    <row r="25" spans="1:4" ht="15">
+      <c r="D24" s="37"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>67</v>
       </c>
@@ -1460,9 +1455,9 @@
       <c r="C25" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="37"/>
-    </row>
-    <row r="26" spans="1:4" ht="15">
+      <c r="D25" s="38"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>70</v>
       </c>
@@ -1472,11 +1467,11 @@
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="41" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>73</v>
       </c>
@@ -1486,9 +1481,9 @@
       <c r="C27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="21"/>
-    </row>
-    <row r="28" spans="1:4" ht="15">
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>75</v>
       </c>
@@ -1498,533 +1493,527 @@
       <c r="C28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:4" ht="15">
-      <c r="A29" s="6" t="s">
+      <c r="D28" s="29"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="30"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="22"/>
-    </row>
-    <row r="30" spans="1:4" ht="15">
-      <c r="A30" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15">
-      <c r="A31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="1:4" ht="15">
+      <c r="D31" s="29"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="22"/>
-    </row>
-    <row r="33" spans="1:9" ht="15">
+      <c r="D32" s="30"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15">
-      <c r="A34" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="1:9" ht="15">
+      <c r="D34" s="29"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="B36" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="D35" s="21"/>
-    </row>
-    <row r="36" spans="1:9" ht="15">
-      <c r="A36" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="21"/>
-    </row>
-    <row r="37" spans="1:9" ht="15">
+      <c r="D36" s="29"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="D37" s="29"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="B38" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:9" ht="15">
-      <c r="A38" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="22"/>
-    </row>
-    <row r="39" spans="1:9" ht="15">
+      <c r="D38" s="30"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15">
-      <c r="A40" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="22"/>
-    </row>
-    <row r="41" spans="1:9" ht="15">
+      <c r="D40" s="30"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="32" t="s">
-        <v>108</v>
+      <c r="D41" s="34" t="s">
+        <v>106</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="21"/>
+      <c r="D42" s="29"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="21"/>
+      <c r="D43" s="29"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="21"/>
-    </row>
-    <row r="45" spans="1:9" ht="15">
+      <c r="D44" s="29"/>
+    </row>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="21"/>
-    </row>
-    <row r="46" spans="1:9" ht="15">
+      <c r="D45" s="29"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:9" ht="15">
+      <c r="D46" s="29"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:9" ht="15">
+      <c r="D47" s="29"/>
+    </row>
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="D48" s="29"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="B49" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="D48" s="21"/>
-    </row>
-    <row r="49" spans="1:4" ht="15">
-      <c r="A49" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="22"/>
-    </row>
-    <row r="50" spans="1:4" ht="15">
+      <c r="D49" s="30"/>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C50" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="33" t="s">
+      <c r="D50" s="44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="15" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15">
-      <c r="A51" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>129</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="21"/>
-    </row>
-    <row r="52" spans="1:4" ht="15">
+      <c r="D51" s="29"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D52" s="21"/>
-    </row>
-    <row r="53" spans="1:4" ht="15">
+      <c r="D52" s="29"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D53" s="22"/>
-    </row>
-    <row r="54" spans="1:4" ht="15">
+      <c r="D53" s="30"/>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="34" t="s">
+      <c r="D54" s="45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="15" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15">
-      <c r="A55" s="14" t="s">
+      <c r="C55" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="D55" s="29"/>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="B56" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="D55" s="21"/>
-    </row>
-    <row r="56" spans="1:4" ht="15">
-      <c r="A56" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>141</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="21"/>
-    </row>
-    <row r="57" spans="1:4" ht="15">
+      <c r="D56" s="29"/>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D57" s="22"/>
-    </row>
-    <row r="58" spans="1:4" ht="15">
+      <c r="D57" s="30"/>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="15" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15">
-      <c r="A59" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>148</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="21"/>
-    </row>
-    <row r="60" spans="1:4" ht="15">
+      <c r="D59" s="29"/>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D60" s="21"/>
-    </row>
-    <row r="61" spans="1:4" ht="15">
+      <c r="D60" s="29"/>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D61" s="21"/>
-    </row>
-    <row r="62" spans="1:4" ht="15">
+      <c r="D61" s="29"/>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C62" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D62" s="21"/>
-    </row>
-    <row r="63" spans="1:4" ht="15">
+      <c r="D62" s="29"/>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="B63" s="15" t="s">
+      <c r="D63" s="30"/>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="B64" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="D63" s="22"/>
-    </row>
-    <row r="64" spans="1:4" ht="15">
-      <c r="A64" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>159</v>
       </c>
       <c r="C64" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D64" s="23" t="s">
+      <c r="D64" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15">
-      <c r="A65" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>162</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D65" s="21"/>
-    </row>
-    <row r="66" spans="1:4" ht="15">
+      <c r="D65" s="29"/>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C66" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D66" s="21"/>
-    </row>
-    <row r="67" spans="1:4" ht="15">
-      <c r="A67" s="38" t="s">
+      <c r="D66" s="29"/>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A67" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" s="29"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B67" s="39" t="s">
+      <c r="B68" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C68" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A69" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="B69" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D67" s="21"/>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A68" s="41" t="s">
+      <c r="D69" s="27"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="B68" s="42" t="s">
+      <c r="B70" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C68" s="43" t="s">
-        <v>170</v>
-      </c>
-      <c r="D68" s="44" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="15">
-      <c r="A69" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="B69" s="42" t="s">
-        <v>173</v>
-      </c>
-      <c r="C69" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" s="45"/>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A70" s="41" t="s">
+      <c r="C70" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B70" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="C70" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="D70" s="45"/>
+      <c r="D70" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>